<commit_message>
Update creation of start and end dates for the study and pregnancy period
</commit_message>
<xml_diff>
--- a/p_steps/parameters/study_dates.xlsx
+++ b/p_steps/parameters/study_dates.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vhoxhaj/Desktop/DP4_Migraine_GitHub/Demonstration project/DP4_Migraine/p_steps/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1279DA46-3495-0545-B1F9-4D5D5A4D14B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FBC04E-7B6F-E249-A418-6903B192F338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15960" xr2:uid="{52957A4A-17C1-3F45-8252-919372C3F876}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="57">
   <si>
     <t>Study</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>20200301</t>
+  </si>
+  <si>
+    <t>This allows only for 3 month look back what about 6 months? Should i change the start_coverage?</t>
   </si>
 </sst>
 </file>
@@ -574,7 +577,7 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -638,6 +641,9 @@
       <c r="G2" s="2">
         <v>0</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
change study dates for CHUT where lookback is set to 2.5month(75.625 days) and after delivery to 0
</commit_message>
<xml_diff>
--- a/p_steps/parameters/study_dates.xlsx
+++ b/p_steps/parameters/study_dates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vhoxhaj/Desktop/DP4_Migraine_GitHub/Demonstration project/DP4_Migraine/p_steps/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9144E87-F05C-C040-83EF-50B25551D82E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9CEEF6-E490-7146-B5A9-B6CD326A560B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="580" windowWidth="28800" windowHeight="16320" xr2:uid="{52957A4A-17C1-3F45-8252-919372C3F876}"/>
   </bookViews>
@@ -178,12 +178,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,7 +503,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B31" sqref="B31"/>
+      <selection pane="topRight" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -568,8 +569,8 @@
       <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2">
-        <v>90.75</v>
+      <c r="G2" s="5">
+        <v>75625</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -725,11 +726,11 @@
       <c r="F8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G8">
-        <v>90.75</v>
+      <c r="G8" s="5">
+        <v>75625</v>
       </c>
       <c r="H8">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -881,8 +882,8 @@
       <c r="F14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G14">
-        <v>90.75</v>
+      <c r="G14" s="5">
+        <v>75625</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1037,8 +1038,8 @@
       <c r="F20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G20">
-        <v>90.75</v>
+      <c r="G20" s="5">
+        <v>75625</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -1196,12 +1197,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004121B7B21A8E79498360E7D69C664CF8" ma:contentTypeVersion="6" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="50fa45a33d7dd66f36eed652322f7e85">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1bb27bd4-d919-4cde-be8f-c8c01880f38f" xmlns:ns3="101111ff-a703-44f4-bedb-571a174d8990" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1aa411700356cc8e21a865bb26eb38d3" ns2:_="" ns3:_="">
     <xsd:import namespace="1bb27bd4-d919-4cde-be8f-c8c01880f38f"/>
@@ -1380,6 +1375,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEF50071-A32A-4A21-9871-71238A273BCA}">
   <ds:schemaRefs>
@@ -1389,23 +1390,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7FAB86A5-2864-4B66-A044-D0381A201D5C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="1bb27bd4-d919-4cde-be8f-c8c01880f38f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="101111ff-a703-44f4-bedb-571a174d8990"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{632FB4B3-1CB8-4DD1-B569-A6F2D6A09D9B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1422,4 +1406,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7FAB86A5-2864-4B66-A044-D0381A201D5C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="1bb27bd4-d919-4cde-be8f-c8c01880f38f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="101111ff-a703-44f4-bedb-571a174d8990"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update timelines for CHUT
</commit_message>
<xml_diff>
--- a/p_steps/parameters/study_dates.xlsx
+++ b/p_steps/parameters/study_dates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vhoxhaj/Desktop/DP4_Migraine_GitHub/Demonstration project/DP4_Migraine/p_steps/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9CEEF6-E490-7146-B5A9-B6CD326A560B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D4E5D4-CB6A-214F-913E-468C74EC4F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="580" windowWidth="28800" windowHeight="16320" xr2:uid="{52957A4A-17C1-3F45-8252-919372C3F876}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{52957A4A-17C1-3F45-8252-919372C3F876}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -178,13 +178,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,26 +501,28 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J11" sqref="J11"/>
+      <selection pane="topRight" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="1"/>
     <col min="3" max="3" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" style="1"/>
+    <col min="9" max="9" width="24.6640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -537,13 +537,13 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J1" t="s">
@@ -551,7 +551,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -569,15 +569,15 @@
       <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="5">
-        <v>75625</v>
-      </c>
-      <c r="H2">
+      <c r="G2" s="1">
+        <v>75.625</v>
+      </c>
+      <c r="H2" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -595,15 +595,15 @@
       <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G3">
-        <v>365.25</v>
-      </c>
-      <c r="H3">
+      <c r="G3" s="1">
+        <v>365.25</v>
+      </c>
+      <c r="H3" s="1">
         <v>90.75</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -621,15 +621,15 @@
       <c r="F4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G4">
-        <v>365.25</v>
-      </c>
-      <c r="H4">
+      <c r="G4" s="1">
+        <v>365.25</v>
+      </c>
+      <c r="H4" s="1">
         <v>90.75</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -647,16 +647,16 @@
       <c r="F5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G5">
-        <v>365.25</v>
-      </c>
-      <c r="H5">
+      <c r="G5" s="1">
+        <v>365.25</v>
+      </c>
+      <c r="H5" s="1">
         <v>90.75</v>
       </c>
-      <c r="J5" s="4"/>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -674,15 +674,15 @@
       <c r="F6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G6">
-        <v>365.25</v>
-      </c>
-      <c r="H6">
+      <c r="G6" s="1">
+        <v>365.25</v>
+      </c>
+      <c r="H6" s="1">
         <v>90.75</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -700,15 +700,15 @@
       <c r="F7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G7">
-        <v>365.25</v>
-      </c>
-      <c r="H7">
+      <c r="G7" s="1">
+        <v>365.25</v>
+      </c>
+      <c r="H7" s="1">
         <v>90.75</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -726,15 +726,15 @@
       <c r="F8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="5">
-        <v>75625</v>
-      </c>
-      <c r="H8">
+      <c r="G8" s="1">
+        <v>75.625</v>
+      </c>
+      <c r="H8" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -752,15 +752,15 @@
       <c r="F9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G9">
-        <v>365.25</v>
-      </c>
-      <c r="H9">
+      <c r="G9" s="1">
+        <v>365.25</v>
+      </c>
+      <c r="H9" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -778,15 +778,15 @@
       <c r="F10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G10">
-        <v>365.25</v>
-      </c>
-      <c r="H10">
+      <c r="G10" s="1">
+        <v>365.25</v>
+      </c>
+      <c r="H10" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -804,15 +804,15 @@
       <c r="F11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G11">
-        <v>365.25</v>
-      </c>
-      <c r="H11">
+      <c r="G11" s="1">
+        <v>365.25</v>
+      </c>
+      <c r="H11" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -830,15 +830,15 @@
       <c r="F12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G12">
-        <v>365.25</v>
-      </c>
-      <c r="H12">
+      <c r="G12" s="1">
+        <v>365.25</v>
+      </c>
+      <c r="H12" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -856,15 +856,15 @@
       <c r="F13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G13">
-        <v>365.25</v>
-      </c>
-      <c r="H13">
+      <c r="G13" s="1">
+        <v>365.25</v>
+      </c>
+      <c r="H13" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -882,15 +882,15 @@
       <c r="F14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="5">
-        <v>75625</v>
-      </c>
-      <c r="H14">
+      <c r="G14" s="1">
+        <v>75.625</v>
+      </c>
+      <c r="H14" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -908,15 +908,15 @@
       <c r="F15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G15">
-        <v>365.25</v>
-      </c>
-      <c r="H15">
+      <c r="G15" s="1">
+        <v>365.25</v>
+      </c>
+      <c r="H15" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -934,15 +934,15 @@
       <c r="F16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G16">
-        <v>365.25</v>
-      </c>
-      <c r="H16">
+      <c r="G16" s="1">
+        <v>365.25</v>
+      </c>
+      <c r="H16" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -960,15 +960,15 @@
       <c r="F17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G17">
-        <v>365.25</v>
-      </c>
-      <c r="H17">
+      <c r="G17" s="1">
+        <v>365.25</v>
+      </c>
+      <c r="H17" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -986,15 +986,15 @@
       <c r="F18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G18">
-        <v>365.25</v>
-      </c>
-      <c r="H18">
+      <c r="G18" s="1">
+        <v>365.25</v>
+      </c>
+      <c r="H18" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1012,15 +1012,15 @@
       <c r="F19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G19">
-        <v>365.25</v>
-      </c>
-      <c r="H19">
+      <c r="G19" s="1">
+        <v>365.25</v>
+      </c>
+      <c r="H19" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -1038,15 +1038,15 @@
       <c r="F20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="5">
-        <v>75625</v>
-      </c>
-      <c r="H20">
+      <c r="G20" s="1">
+        <v>75.625</v>
+      </c>
+      <c r="H20" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -1064,15 +1064,15 @@
       <c r="F21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G21">
-        <v>365.25</v>
-      </c>
-      <c r="H21">
+      <c r="G21" s="1">
+        <v>365.25</v>
+      </c>
+      <c r="H21" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1090,15 +1090,15 @@
       <c r="F22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G22">
-        <v>365.25</v>
-      </c>
-      <c r="H22">
+      <c r="G22" s="1">
+        <v>365.25</v>
+      </c>
+      <c r="H22" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1116,15 +1116,15 @@
       <c r="F23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G23">
-        <v>365.25</v>
-      </c>
-      <c r="H23">
+      <c r="G23" s="1">
+        <v>365.25</v>
+      </c>
+      <c r="H23" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -1142,15 +1142,15 @@
       <c r="F24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G24">
-        <v>365.25</v>
-      </c>
-      <c r="H24">
+      <c r="G24" s="1">
+        <v>365.25</v>
+      </c>
+      <c r="H24" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -1168,10 +1168,10 @@
       <c r="F25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G25">
-        <v>365.25</v>
-      </c>
-      <c r="H25">
+      <c r="G25" s="1">
+        <v>365.25</v>
+      </c>
+      <c r="H25" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1188,12 +1188,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1376,15 +1373,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEF50071-A32A-4A21-9871-71238A273BCA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7FAB86A5-2864-4B66-A044-D0381A201D5C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="1bb27bd4-d919-4cde-be8f-c8c01880f38f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="101111ff-a703-44f4-bedb-571a174d8990"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1409,18 +1418,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7FAB86A5-2864-4B66-A044-D0381A201D5C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEF50071-A32A-4A21-9871-71238A273BCA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="1bb27bd4-d919-4cde-be8f-c8c01880f38f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="101111ff-a703-44f4-bedb-571a174d8990"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>